<commit_message>
initial working version /19Sept
</commit_message>
<xml_diff>
--- a/items/آویز گردنبند طلا 18 عیار زنانه.xlsx
+++ b/items/آویز گردنبند طلا 18 عیار زنانه.xlsx
@@ -1,17 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
-  <workbookPr defaultThemeVersion="164011" filterPrivacy="1"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24332"/>
+  <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1424C6CB-8C9B-4516-9008-B34B10E4F4FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <bookViews>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+  </bookViews>
   <sheets>
-    <sheet sheetId="1" name="Sheet 1" state="visible" r:id="rId4"/>
+    <sheet name="Sheet 1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="171027"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>Date</t>
   </si>
@@ -34,14 +38,14 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-      <sz val="11"/>
-      <name val="Calibri"/>
     </font>
   </fonts>
   <fills count="2">
@@ -404,9 +408,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C3"/>
-  <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:XFD2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
@@ -430,19 +439,8 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3" t="s">
-        <v>4</v>
-      </c>
-      <c r="C3" t="s">
-        <v>5</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1" firstPageNumber="1" useFirstPageNumber="1" copies="1"/>
+  <pageSetup orientation="portrait" useFirstPageNumber="1" horizontalDpi="4294967295" verticalDpi="4294967295"/>
 </worksheet>
 </file>
</xml_diff>